<commit_message>
Punto 2 resuelto delegando: Hogwards -> Casa -> estudiante.getEspecie
</commit_message>
<xml_diff>
--- a/HarryPotter-data.xlsx
+++ b/HarryPotter-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nasaban\IdeaProjects\arpro.grupo11.harrypotter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22CDAEF-2C37-4564-B050-DD0A4AD87E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EC89D4-5676-4422-822D-C55AA4BBC50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$141</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1074,6 +1074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1114,7 +1115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1137,7 +1138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1229,7 +1230,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1252,7 +1253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1275,7 +1276,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1298,7 +1299,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1321,7 +1322,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1344,7 +1345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1367,7 +1368,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1450,7 +1451,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1473,7 +1474,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1519,7 +1520,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1611,7 +1612,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1634,7 +1635,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1726,7 +1727,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1749,7 +1750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1815,7 +1816,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1838,7 +1839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1861,7 +1862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1884,7 +1885,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1907,7 +1908,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1953,7 +1954,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1976,7 +1977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2022,7 +2023,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2045,7 +2046,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2068,7 +2069,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2091,7 +2092,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2114,7 +2115,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2137,7 +2138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2249,7 +2250,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2272,7 +2273,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2292,7 +2293,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2378,7 +2379,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2401,7 +2402,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2447,7 +2448,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2490,7 +2491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2536,7 +2537,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2559,7 +2560,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2582,7 +2583,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2628,7 +2629,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2651,7 +2652,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2674,7 +2675,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2717,7 +2718,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2734,7 +2735,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2754,7 +2755,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2774,7 +2775,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2791,7 +2792,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2814,7 +2815,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2903,7 +2904,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2926,7 +2927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2972,7 +2973,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2995,7 +2996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3041,7 +3042,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3064,7 +3065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3110,7 +3111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3156,7 +3157,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3179,7 +3180,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3202,7 +3203,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3242,7 +3243,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3262,7 +3263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3282,7 +3283,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3305,7 +3306,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3322,7 +3323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3342,7 +3343,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3362,7 +3363,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3382,7 +3383,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3399,7 +3400,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3419,7 +3420,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3442,7 +3443,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3462,7 +3463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3482,7 +3483,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3502,7 +3503,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3522,7 +3523,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3536,7 +3537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3553,7 +3554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3570,7 +3571,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3587,7 +3588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3607,7 +3608,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3621,7 +3622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3635,7 +3636,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3658,7 +3659,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3678,7 +3679,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3701,7 +3702,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3718,7 +3719,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3738,7 +3739,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3755,7 +3756,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3775,7 +3776,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3798,7 +3799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3821,7 +3822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3867,7 +3868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3890,7 +3891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3913,7 +3914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3933,7 +3934,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3953,7 +3954,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3970,7 +3971,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3987,7 +3988,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4007,7 +4008,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4024,7 +4025,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4041,7 +4042,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4055,7 +4056,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4075,7 +4076,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4092,7 +4093,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4110,7 +4111,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G141" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Gryffindor"/>
+        <filter val="Hufflepuff"/>
+        <filter val="Ravenclaw"/>
+        <filter val="Slytherin"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Centaur"/>
+        <filter val="elf"/>
+        <filter val="Ghost"/>
+        <filter val="Half-Human/Half-Giant"/>
+        <filter val="Human (Metamorphmagus)"/>
+        <filter val="Human (Werewolf traits)"/>
+        <filter val="Human(goblin ancestry)"/>
+        <filter val="Werewolf"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor, punto 1 y 2.
</commit_message>
<xml_diff>
--- a/HarryPotter-data.xlsx
+++ b/HarryPotter-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nasaban\IdeaProjects\arpro.grupo11.harrypotter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EC89D4-5676-4422-822D-C55AA4BBC50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB439850-E60E-4F5C-9441-99FF46619480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1078,7 +1078,7 @@
   <dimension ref="A1:G141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4112,6 +4112,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G141" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Student"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters>
         <filter val="Gryffindor"/>
@@ -4122,8 +4127,6 @@
     </filterColumn>
     <filterColumn colId="5">
       <filters>
-        <filter val="Centaur"/>
-        <filter val="elf"/>
         <filter val="Ghost"/>
         <filter val="Half-Human/Half-Giant"/>
         <filter val="Human (Metamorphmagus)"/>

</xml_diff>